<commit_message>
The necessary test class and XML file for parallel testing have been created. In addition, adjustments have been made to our existing classes for parallel execution.
</commit_message>
<xml_diff>
--- a/AppiumPOM_02/src/test/resources/testdata.xlsx
+++ b/AppiumPOM_02/src/test/resources/testdata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fab46644dc17b22/Desktop/Appium Examples/AppiumPOM_02/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{65C2C96C-8299-4EE5-900F-AEB22562E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E008F03-69BA-4C82-84E6-24548FFB5BBE}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{65C2C96C-8299-4EE5-900F-AEB22562E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17764AF-04F8-4A1D-96F7-E9C0E09F1C72}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E0DF160F-E992-4E58-8AC1-1823EDAC366F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{E0DF160F-E992-4E58-8AC1-1823EDAC366F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="ParallelLoginData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>TestCase</t>
   </si>
@@ -84,6 +86,9 @@
   </si>
   <si>
     <t>wrongpass</t>
+  </si>
+  <si>
+    <t>wronguserexample.com</t>
   </si>
 </sst>
 </file>
@@ -144,6 +149,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED9F10A-338D-4121-879B-6E779BCA0BD9}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="B1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,4 +563,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC191452-0A3B-4F66-9DF9-151759BA0B30}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6B5A32-3FB7-40A5-BCB3-09D29DA4D617}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SearchTest has been added and BaseTest has been added for static tests. For parallel test we have to use BaseTestParallelTest class.
</commit_message>
<xml_diff>
--- a/AppiumPOM_02/src/test/resources/testdata.xlsx
+++ b/AppiumPOM_02/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fab46644dc17b22/Desktop/Appium Examples/AppiumPOM_02/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{65C2C96C-8299-4EE5-900F-AEB22562E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17764AF-04F8-4A1D-96F7-E9C0E09F1C72}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{65C2C96C-8299-4EE5-900F-AEB22562E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38DF0474-5596-4ED3-8916-289AA5262225}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{E0DF160F-E992-4E58-8AC1-1823EDAC366F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E0DF160F-E992-4E58-8AC1-1823EDAC366F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>TestCase</t>
   </si>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC191452-0A3B-4F66-9DF9-151759BA0B30}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,20 +604,15 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -630,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6B5A32-3FB7-40A5-BCB3-09D29DA4D617}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>